<commit_message>
Fixing the Results Consumption Export
</commit_message>
<xml_diff>
--- a/RAAL/Consumption/Results_Consumption_RAAL.xlsx
+++ b/RAAL/Consumption/Results_Consumption_RAAL.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mynexte-my.sharepoint.com/personal/andrei_ionita_mynexte_com/Documents/Desktop/ML/Forecast_app/RAAL/Consumption/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_574E8703C501D318C4070311FCAB83076B40B28D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{01D8C7EB-22DB-4E31-AE37-1349D9AE78ED}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Consumption_Predictions" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -28,11 +34,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="dd.mm.yyyy"/>
+    <numFmt numFmtId="164" formatCode="dd\.mm\.yyyy"/>
   </numFmts>
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -70,13 +76,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -114,7 +128,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -148,6 +162,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -182,9 +197,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -357,14 +373,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C145"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N13" sqref="N13"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -375,7 +396,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>45269</v>
       </c>
@@ -386,7 +407,7 @@
         <v>1.771760106086731</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>45269</v>
       </c>
@@ -394,10 +415,10 @@
         <v>1</v>
       </c>
       <c r="C3">
-        <v>1.750019192695618</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
+        <v>1.7500191926956179</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>45269</v>
       </c>
@@ -408,7 +429,7 @@
         <v>1.633675217628479</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>45269</v>
       </c>
@@ -419,7 +440,7 @@
         <v>1.631011843681335</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>45269</v>
       </c>
@@ -430,7 +451,7 @@
         <v>1.631011843681335</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>45269</v>
       </c>
@@ -441,7 +462,7 @@
         <v>1.798055171966553</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>45269</v>
       </c>
@@ -449,10 +470,10 @@
         <v>6</v>
       </c>
       <c r="C8">
-        <v>1.886846899986267</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
+        <v>1.8868468999862671</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>45269</v>
       </c>
@@ -460,10 +481,10 @@
         <v>7</v>
       </c>
       <c r="C9">
-        <v>2.188735246658325</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
+        <v>2.1887352466583252</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>45269</v>
       </c>
@@ -471,10 +492,10 @@
         <v>8</v>
       </c>
       <c r="C10">
-        <v>2.179297685623169</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
+        <v>2.1792976856231689</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>45269</v>
       </c>
@@ -485,7 +506,7 @@
         <v>2.115292072296143</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>45269</v>
       </c>
@@ -493,10 +514,10 @@
         <v>10</v>
       </c>
       <c r="C12">
-        <v>2.386186361312866</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
+        <v>2.3861863613128662</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>45269</v>
       </c>
@@ -504,10 +525,10 @@
         <v>11</v>
       </c>
       <c r="C13">
-        <v>2.033339738845825</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
+        <v>2.0333397388458252</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>45269</v>
       </c>
@@ -515,10 +536,10 @@
         <v>12</v>
       </c>
       <c r="C14">
-        <v>1.28935980796814</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
+        <v>1.2893598079681401</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>45269</v>
       </c>
@@ -526,10 +547,10 @@
         <v>13</v>
       </c>
       <c r="C15">
-        <v>0.9899243712425232</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
+        <v>0.98992437124252319</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>45269</v>
       </c>
@@ -537,10 +558,10 @@
         <v>14</v>
       </c>
       <c r="C16">
-        <v>0.722099244594574</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
+        <v>0.72209924459457397</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>45269</v>
       </c>
@@ -548,10 +569,10 @@
         <v>15</v>
       </c>
       <c r="C17">
-        <v>0.6323621869087219</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
+        <v>0.63236218690872192</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>45269</v>
       </c>
@@ -559,10 +580,10 @@
         <v>16</v>
       </c>
       <c r="C18">
-        <v>0.6869106888771057</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
+        <v>0.68691068887710571</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>45269</v>
       </c>
@@ -570,10 +591,10 @@
         <v>17</v>
       </c>
       <c r="C19">
-        <v>0.5752869844436646</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
+        <v>0.57528698444366455</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>45269</v>
       </c>
@@ -581,10 +602,10 @@
         <v>18</v>
       </c>
       <c r="C20">
-        <v>0.5696507692337036</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
+        <v>0.56965076923370361</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>45269</v>
       </c>
@@ -592,10 +613,10 @@
         <v>19</v>
       </c>
       <c r="C21">
-        <v>0.5790761709213257</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3">
+        <v>0.57907617092132568</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>45269</v>
       </c>
@@ -603,10 +624,10 @@
         <v>20</v>
       </c>
       <c r="C22">
-        <v>0.572188675403595</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3">
+        <v>0.57218867540359497</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>45269</v>
       </c>
@@ -614,10 +635,10 @@
         <v>21</v>
       </c>
       <c r="C23">
-        <v>0.572188675403595</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3">
+        <v>0.57218867540359497</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>45269</v>
       </c>
@@ -625,10 +646,10 @@
         <v>22</v>
       </c>
       <c r="C24">
-        <v>0.5648350119590759</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3">
+        <v>0.56483501195907593</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>45269</v>
       </c>
@@ -636,10 +657,10 @@
         <v>23</v>
       </c>
       <c r="C25">
-        <v>0.5648350119590759</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3">
+        <v>0.56483501195907593</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>45270</v>
       </c>
@@ -647,10 +668,10 @@
         <v>0</v>
       </c>
       <c r="C26">
-        <v>0.6276118755340576</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3">
+        <v>0.62761187553405762</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>45270</v>
       </c>
@@ -658,10 +679,10 @@
         <v>1</v>
       </c>
       <c r="C27">
-        <v>0.6276118755340576</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3">
+        <v>0.62761187553405762</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>45270</v>
       </c>
@@ -669,10 +690,10 @@
         <v>2</v>
       </c>
       <c r="C28">
-        <v>0.6236113309860229</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3">
+        <v>0.62361133098602295</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>45270</v>
       </c>
@@ -680,10 +701,10 @@
         <v>3</v>
       </c>
       <c r="C29">
-        <v>0.6236113309860229</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3">
+        <v>0.62361133098602295</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>45270</v>
       </c>
@@ -691,10 +712,10 @@
         <v>4</v>
       </c>
       <c r="C30">
-        <v>0.6236113309860229</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3">
+        <v>0.62361133098602295</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>45270</v>
       </c>
@@ -702,10 +723,10 @@
         <v>5</v>
       </c>
       <c r="C31">
-        <v>0.6231423616409302</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3">
+        <v>0.62314236164093018</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>45270</v>
       </c>
@@ -713,10 +734,10 @@
         <v>6</v>
       </c>
       <c r="C32">
-        <v>0.6231423616409302</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3">
+        <v>0.62314236164093018</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>45270</v>
       </c>
@@ -727,7 +748,7 @@
         <v>0.6294858455657959</v>
       </c>
     </row>
-    <row r="34" spans="1:3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>45270</v>
       </c>
@@ -735,10 +756,10 @@
         <v>8</v>
       </c>
       <c r="C34">
-        <v>0.6346346139907837</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3">
+        <v>0.63463461399078369</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>45270</v>
       </c>
@@ -746,10 +767,10 @@
         <v>9</v>
       </c>
       <c r="C35">
-        <v>0.6346346139907837</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3">
+        <v>0.63463461399078369</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>45270</v>
       </c>
@@ -757,10 +778,10 @@
         <v>10</v>
       </c>
       <c r="C36">
-        <v>0.7153280377388</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3">
+        <v>0.71532803773880005</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>45270</v>
       </c>
@@ -768,10 +789,10 @@
         <v>11</v>
       </c>
       <c r="C37">
-        <v>0.7049685120582581</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3">
+        <v>0.70496851205825806</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>45270</v>
       </c>
@@ -779,10 +800,10 @@
         <v>12</v>
       </c>
       <c r="C38">
-        <v>0.6954421401023865</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3">
+        <v>0.69544214010238647</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>45270</v>
       </c>
@@ -790,10 +811,10 @@
         <v>13</v>
       </c>
       <c r="C39">
-        <v>0.6954421401023865</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3">
+        <v>0.69544214010238647</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>45270</v>
       </c>
@@ -801,10 +822,10 @@
         <v>14</v>
       </c>
       <c r="C40">
-        <v>0.7019732594490051</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3">
+        <v>0.70197325944900513</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>45270</v>
       </c>
@@ -812,10 +833,10 @@
         <v>15</v>
       </c>
       <c r="C41">
-        <v>0.7048743367195129</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3">
+        <v>0.70487433671951294</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>45270</v>
       </c>
@@ -823,10 +844,10 @@
         <v>16</v>
       </c>
       <c r="C42">
-        <v>0.7225372195243835</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3">
+        <v>0.72253721952438354</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>45270</v>
       </c>
@@ -834,10 +855,10 @@
         <v>17</v>
       </c>
       <c r="C43">
-        <v>0.7225372195243835</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3">
+        <v>0.72253721952438354</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>45270</v>
       </c>
@@ -845,10 +866,10 @@
         <v>18</v>
       </c>
       <c r="C44">
-        <v>0.6533039808273315</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3">
+        <v>0.65330398082733154</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>45270</v>
       </c>
@@ -856,10 +877,10 @@
         <v>19</v>
       </c>
       <c r="C45">
-        <v>0.6627293825149536</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3">
+        <v>0.66272938251495361</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>45270</v>
       </c>
@@ -870,7 +891,7 @@
         <v>0.6558418869972229</v>
       </c>
     </row>
-    <row r="47" spans="1:3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>45270</v>
       </c>
@@ -881,7 +902,7 @@
         <v>0.6558418869972229</v>
       </c>
     </row>
-    <row r="48" spans="1:3">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>45270</v>
       </c>
@@ -892,7 +913,7 @@
         <v>0.6464572548866272</v>
       </c>
     </row>
-    <row r="49" spans="1:3">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>45270</v>
       </c>
@@ -903,7 +924,7 @@
         <v>0.6464572548866272</v>
       </c>
     </row>
-    <row r="50" spans="1:3">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>45271</v>
       </c>
@@ -911,10 +932,10 @@
         <v>0</v>
       </c>
       <c r="C50">
-        <v>0.8702195286750793</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3">
+        <v>0.87021952867507935</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>45271</v>
       </c>
@@ -922,10 +943,10 @@
         <v>1</v>
       </c>
       <c r="C51">
-        <v>0.9694542288780212</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3">
+        <v>0.96945422887802124</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>45271</v>
       </c>
@@ -933,10 +954,10 @@
         <v>2</v>
       </c>
       <c r="C52">
-        <v>1.041930794715881</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3">
+        <v>1.0419307947158809</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>45271</v>
       </c>
@@ -944,10 +965,10 @@
         <v>3</v>
       </c>
       <c r="C53">
-        <v>1.275074481964111</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3">
+        <v>1.2750744819641111</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>45271</v>
       </c>
@@ -958,7 +979,7 @@
         <v>1.562673807144165</v>
       </c>
     </row>
-    <row r="55" spans="1:3">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>45271</v>
       </c>
@@ -969,7 +990,7 @@
         <v>1.936149120330811</v>
       </c>
     </row>
-    <row r="56" spans="1:3">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>45271</v>
       </c>
@@ -980,7 +1001,7 @@
         <v>2.18621826171875</v>
       </c>
     </row>
-    <row r="57" spans="1:3">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>45271</v>
       </c>
@@ -988,10 +1009,10 @@
         <v>7</v>
       </c>
       <c r="C57">
-        <v>3.803076982498169</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3">
+        <v>3.8030769824981689</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>45271</v>
       </c>
@@ -999,10 +1020,10 @@
         <v>8</v>
       </c>
       <c r="C58">
-        <v>4.229624271392822</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3">
+        <v>4.2296242713928223</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>45271</v>
       </c>
@@ -1013,7 +1034,7 @@
         <v>4.224860668182373</v>
       </c>
     </row>
-    <row r="60" spans="1:3">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>45271</v>
       </c>
@@ -1021,10 +1042,10 @@
         <v>10</v>
       </c>
       <c r="C60">
-        <v>4.134963512420654</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3">
+        <v>4.1349635124206543</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>45271</v>
       </c>
@@ -1032,10 +1053,10 @@
         <v>11</v>
       </c>
       <c r="C61">
-        <v>3.599840879440308</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3">
+        <v>3.5998408794403081</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>45271</v>
       </c>
@@ -1043,10 +1064,10 @@
         <v>12</v>
       </c>
       <c r="C62">
-        <v>3.88855767250061</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3">
+        <v>3.8885576725006099</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>45271</v>
       </c>
@@ -1054,10 +1075,10 @@
         <v>13</v>
       </c>
       <c r="C63">
-        <v>3.886303663253784</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3">
+        <v>3.8863036632537842</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>45271</v>
       </c>
@@ -1068,7 +1089,7 @@
         <v>3.368045568466187</v>
       </c>
     </row>
-    <row r="65" spans="1:3">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>45271</v>
       </c>
@@ -1076,10 +1097,10 @@
         <v>15</v>
       </c>
       <c r="C65">
-        <v>3.243540287017822</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3">
+        <v>3.2435402870178218</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>45271</v>
       </c>
@@ -1087,10 +1108,10 @@
         <v>16</v>
       </c>
       <c r="C66">
-        <v>3.331707954406738</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3">
+        <v>3.3317079544067378</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>45271</v>
       </c>
@@ -1098,10 +1119,10 @@
         <v>17</v>
       </c>
       <c r="C67">
-        <v>3.133861064910889</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3">
+        <v>3.1338610649108891</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>45271</v>
       </c>
@@ -1109,10 +1130,10 @@
         <v>18</v>
       </c>
       <c r="C68">
-        <v>3.441512107849121</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3">
+        <v>3.4415121078491211</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>45271</v>
       </c>
@@ -1120,10 +1141,10 @@
         <v>19</v>
       </c>
       <c r="C69">
-        <v>3.261330604553223</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3">
+        <v>3.2613306045532231</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>45271</v>
       </c>
@@ -1131,10 +1152,10 @@
         <v>20</v>
       </c>
       <c r="C70">
-        <v>3.113126993179321</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3">
+        <v>3.1131269931793208</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>45271</v>
       </c>
@@ -1142,10 +1163,10 @@
         <v>21</v>
       </c>
       <c r="C71">
-        <v>3.198132276535034</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3">
+        <v>3.1981322765350342</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>45271</v>
       </c>
@@ -1153,10 +1174,10 @@
         <v>22</v>
       </c>
       <c r="C72">
-        <v>2.688216209411621</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3">
+        <v>2.6882162094116211</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>45271</v>
       </c>
@@ -1167,7 +1188,7 @@
         <v>2.043851375579834</v>
       </c>
     </row>
-    <row r="74" spans="1:3">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>45272</v>
       </c>
@@ -1175,10 +1196,10 @@
         <v>0</v>
       </c>
       <c r="C74">
-        <v>2.112542629241943</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3">
+        <v>2.1125426292419429</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>45272</v>
       </c>
@@ -1186,10 +1207,10 @@
         <v>1</v>
       </c>
       <c r="C75">
-        <v>2.070881366729736</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3">
+        <v>2.0708813667297359</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>45272</v>
       </c>
@@ -1197,10 +1218,10 @@
         <v>2</v>
       </c>
       <c r="C76">
-        <v>2.038943529129028</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3">
+        <v>2.0389435291290279</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>45272</v>
       </c>
@@ -1208,10 +1229,10 @@
         <v>3</v>
       </c>
       <c r="C77">
-        <v>1.994740128517151</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3">
+        <v>1.9947401285171511</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>45272</v>
       </c>
@@ -1219,10 +1240,10 @@
         <v>4</v>
       </c>
       <c r="C78">
-        <v>2.037106513977051</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3">
+        <v>2.0371065139770508</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <v>45272</v>
       </c>
@@ -1233,7 +1254,7 @@
         <v>2.737796306610107</v>
       </c>
     </row>
-    <row r="80" spans="1:3">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>45272</v>
       </c>
@@ -1241,10 +1262,10 @@
         <v>6</v>
       </c>
       <c r="C80">
-        <v>2.874032974243164</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3">
+        <v>2.8740329742431641</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <v>45272</v>
       </c>
@@ -1252,10 +1273,10 @@
         <v>7</v>
       </c>
       <c r="C81">
-        <v>3.903116703033447</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3">
+        <v>3.9031167030334468</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <v>45272</v>
       </c>
@@ -1266,7 +1287,7 @@
         <v>4.041816234588623</v>
       </c>
     </row>
-    <row r="83" spans="1:3">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <v>45272</v>
       </c>
@@ -1277,7 +1298,7 @@
         <v>4.041816234588623</v>
       </c>
     </row>
-    <row r="84" spans="1:3">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <v>45272</v>
       </c>
@@ -1285,10 +1306,10 @@
         <v>10</v>
       </c>
       <c r="C84">
-        <v>4.053033828735352</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3">
+        <v>4.0530338287353516</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <v>45272</v>
       </c>
@@ -1299,7 +1320,7 @@
         <v>3.494188547134399</v>
       </c>
     </row>
-    <row r="86" spans="1:3">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
         <v>45272</v>
       </c>
@@ -1310,7 +1331,7 @@
         <v>3.823432445526123</v>
       </c>
     </row>
-    <row r="87" spans="1:3">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
         <v>45272</v>
       </c>
@@ -1318,10 +1339,10 @@
         <v>13</v>
       </c>
       <c r="C87">
-        <v>3.821178436279297</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3">
+        <v>3.8211784362792969</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
         <v>45272</v>
       </c>
@@ -1329,10 +1350,10 @@
         <v>14</v>
       </c>
       <c r="C88">
-        <v>3.202015161514282</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3">
+        <v>3.2020151615142818</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
         <v>45272</v>
       </c>
@@ -1343,7 +1364,7 @@
         <v>3.077509880065918</v>
       </c>
     </row>
-    <row r="90" spans="1:3">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
         <v>45272</v>
       </c>
@@ -1351,10 +1372,10 @@
         <v>16</v>
       </c>
       <c r="C90">
-        <v>3.201891899108887</v>
-      </c>
-    </row>
-    <row r="91" spans="1:3">
+        <v>3.2018918991088872</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
         <v>45272</v>
       </c>
@@ -1362,10 +1383,10 @@
         <v>17</v>
       </c>
       <c r="C91">
-        <v>3.275767087936401</v>
-      </c>
-    </row>
-    <row r="92" spans="1:3">
+        <v>3.2757670879364009</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
         <v>45272</v>
       </c>
@@ -1373,10 +1394,10 @@
         <v>18</v>
       </c>
       <c r="C92">
-        <v>3.186712026596069</v>
-      </c>
-    </row>
-    <row r="93" spans="1:3">
+        <v>3.1867120265960689</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
         <v>45272</v>
       </c>
@@ -1387,7 +1408,7 @@
         <v>3.097163200378418</v>
       </c>
     </row>
-    <row r="94" spans="1:3">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
         <v>45272</v>
       </c>
@@ -1395,10 +1416,10 @@
         <v>20</v>
       </c>
       <c r="C94">
-        <v>3.191830635070801</v>
-      </c>
-    </row>
-    <row r="95" spans="1:3">
+        <v>3.1918306350708008</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
         <v>45272</v>
       </c>
@@ -1406,10 +1427,10 @@
         <v>21</v>
       </c>
       <c r="C95">
-        <v>2.959413766860962</v>
-      </c>
-    </row>
-    <row r="96" spans="1:3">
+        <v>2.9594137668609619</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
         <v>45272</v>
       </c>
@@ -1417,10 +1438,10 @@
         <v>22</v>
       </c>
       <c r="C96">
-        <v>2.6103835105896</v>
-      </c>
-    </row>
-    <row r="97" spans="1:3">
+        <v>2.6103835105896001</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
         <v>45272</v>
       </c>
@@ -1428,10 +1449,10 @@
         <v>23</v>
       </c>
       <c r="C97">
-        <v>2.128123760223389</v>
-      </c>
-    </row>
-    <row r="98" spans="1:3">
+        <v>2.1281237602233891</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
         <v>45273</v>
       </c>
@@ -1439,10 +1460,10 @@
         <v>0</v>
       </c>
       <c r="C98">
-        <v>2.196894884109497</v>
-      </c>
-    </row>
-    <row r="99" spans="1:3">
+        <v>2.1968948841094971</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
         <v>45273</v>
       </c>
@@ -1453,7 +1474,7 @@
         <v>2.174203634262085</v>
       </c>
     </row>
-    <row r="100" spans="1:3">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
         <v>45273</v>
       </c>
@@ -1464,7 +1485,7 @@
         <v>2.080328226089478</v>
       </c>
     </row>
-    <row r="101" spans="1:3">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
         <v>45273</v>
       </c>
@@ -1475,7 +1496,7 @@
         <v>2.026740550994873</v>
       </c>
     </row>
-    <row r="102" spans="1:3">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
         <v>45273</v>
       </c>
@@ -1483,10 +1504,10 @@
         <v>4</v>
       </c>
       <c r="C102">
-        <v>2.106083631515503</v>
-      </c>
-    </row>
-    <row r="103" spans="1:3">
+        <v>2.1060836315155029</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" s="1">
         <v>45273</v>
       </c>
@@ -1494,10 +1515,10 @@
         <v>5</v>
       </c>
       <c r="C103">
-        <v>2.759424686431885</v>
-      </c>
-    </row>
-    <row r="104" spans="1:3">
+        <v>2.7594246864318852</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" s="1">
         <v>45273</v>
       </c>
@@ -1505,10 +1526,10 @@
         <v>6</v>
       </c>
       <c r="C104">
-        <v>2.903120040893555</v>
-      </c>
-    </row>
-    <row r="105" spans="1:3">
+        <v>2.9031200408935551</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" s="1">
         <v>45273</v>
       </c>
@@ -1516,10 +1537,10 @@
         <v>7</v>
       </c>
       <c r="C105">
-        <v>3.643650531768799</v>
-      </c>
-    </row>
-    <row r="106" spans="1:3">
+        <v>3.6436505317687988</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" s="1">
         <v>45273</v>
       </c>
@@ -1527,10 +1548,10 @@
         <v>8</v>
       </c>
       <c r="C106">
-        <v>3.664962291717529</v>
-      </c>
-    </row>
-    <row r="107" spans="1:3">
+        <v>3.6649622917175289</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" s="1">
         <v>45273</v>
       </c>
@@ -1538,10 +1559,10 @@
         <v>9</v>
       </c>
       <c r="C107">
-        <v>3.716184616088867</v>
-      </c>
-    </row>
-    <row r="108" spans="1:3">
+        <v>3.7161846160888672</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" s="1">
         <v>45273</v>
       </c>
@@ -1549,10 +1570,10 @@
         <v>10</v>
       </c>
       <c r="C108">
-        <v>3.730091094970703</v>
-      </c>
-    </row>
-    <row r="109" spans="1:3">
+        <v>3.7300910949707031</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" s="1">
         <v>45273</v>
       </c>
@@ -1563,7 +1584,7 @@
         <v>3.386167049407959</v>
       </c>
     </row>
-    <row r="110" spans="1:3">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" s="1">
         <v>45273</v>
       </c>
@@ -1571,10 +1592,10 @@
         <v>12</v>
       </c>
       <c r="C110">
-        <v>3.330824136734009</v>
-      </c>
-    </row>
-    <row r="111" spans="1:3">
+        <v>3.3308241367340088</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" s="1">
         <v>45273</v>
       </c>
@@ -1582,10 +1603,10 @@
         <v>13</v>
       </c>
       <c r="C111">
-        <v>3.330824136734009</v>
-      </c>
-    </row>
-    <row r="112" spans="1:3">
+        <v>3.3308241367340088</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" s="1">
         <v>45273</v>
       </c>
@@ -1593,10 +1614,10 @@
         <v>14</v>
       </c>
       <c r="C112">
-        <v>3.076342821121216</v>
-      </c>
-    </row>
-    <row r="113" spans="1:3">
+        <v>3.0763428211212158</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" s="1">
         <v>45273</v>
       </c>
@@ -1607,7 +1628,7 @@
         <v>3.034182071685791</v>
       </c>
     </row>
-    <row r="114" spans="1:3">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" s="1">
         <v>45273</v>
       </c>
@@ -1615,10 +1636,10 @@
         <v>16</v>
       </c>
       <c r="C114">
-        <v>3.233547210693359</v>
-      </c>
-    </row>
-    <row r="115" spans="1:3">
+        <v>3.2335472106933589</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" s="1">
         <v>45273</v>
       </c>
@@ -1626,10 +1647,10 @@
         <v>17</v>
       </c>
       <c r="C115">
-        <v>3.457921743392944</v>
-      </c>
-    </row>
-    <row r="116" spans="1:3">
+        <v>3.4579217433929439</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" s="1">
         <v>45273</v>
       </c>
@@ -1637,10 +1658,10 @@
         <v>18</v>
       </c>
       <c r="C116">
-        <v>3.420974016189575</v>
-      </c>
-    </row>
-    <row r="117" spans="1:3">
+        <v>3.4209740161895752</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" s="1">
         <v>45273</v>
       </c>
@@ -1648,10 +1669,10 @@
         <v>19</v>
       </c>
       <c r="C117">
-        <v>3.209006071090698</v>
-      </c>
-    </row>
-    <row r="118" spans="1:3">
+        <v>3.2090060710906978</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" s="1">
         <v>45273</v>
       </c>
@@ -1659,10 +1680,10 @@
         <v>20</v>
       </c>
       <c r="C118">
-        <v>3.316859722137451</v>
-      </c>
-    </row>
-    <row r="119" spans="1:3">
+        <v>3.3168597221374512</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" s="1">
         <v>45273</v>
       </c>
@@ -1670,10 +1691,10 @@
         <v>21</v>
       </c>
       <c r="C119">
-        <v>3.069310426712036</v>
-      </c>
-    </row>
-    <row r="120" spans="1:3">
+        <v>3.0693104267120361</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" s="1">
         <v>45273</v>
       </c>
@@ -1684,7 +1705,7 @@
         <v>2.671992301940918</v>
       </c>
     </row>
-    <row r="121" spans="1:3">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" s="1">
         <v>45273</v>
       </c>
@@ -1692,10 +1713,10 @@
         <v>23</v>
       </c>
       <c r="C121">
-        <v>2.110560655593872</v>
-      </c>
-    </row>
-    <row r="122" spans="1:3">
+        <v>2.1105606555938721</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" s="1">
         <v>45274</v>
       </c>
@@ -1703,10 +1724,10 @@
         <v>0</v>
       </c>
       <c r="C122">
-        <v>1.726493954658508</v>
-      </c>
-    </row>
-    <row r="123" spans="1:3">
+        <v>1.7264939546585081</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123" s="1">
         <v>45274</v>
       </c>
@@ -1714,10 +1735,10 @@
         <v>1</v>
       </c>
       <c r="C123">
-        <v>1.703802943229675</v>
-      </c>
-    </row>
-    <row r="124" spans="1:3">
+        <v>1.7038029432296751</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124" s="1">
         <v>45274</v>
       </c>
@@ -1725,10 +1746,10 @@
         <v>2</v>
       </c>
       <c r="C124">
-        <v>1.623984336853027</v>
-      </c>
-    </row>
-    <row r="125" spans="1:3">
+        <v>1.6239843368530269</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125" s="1">
         <v>45274</v>
       </c>
@@ -1736,10 +1757,10 @@
         <v>3</v>
       </c>
       <c r="C125">
-        <v>1.580211043357849</v>
-      </c>
-    </row>
-    <row r="126" spans="1:3">
+        <v>1.5802110433578489</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" s="1">
         <v>45274</v>
       </c>
@@ -1747,10 +1768,10 @@
         <v>4</v>
       </c>
       <c r="C126">
-        <v>1.274391531944275</v>
-      </c>
-    </row>
-    <row r="127" spans="1:3">
+        <v>1.2743915319442749</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" s="1">
         <v>45274</v>
       </c>
@@ -1758,10 +1779,10 @@
         <v>5</v>
       </c>
       <c r="C127">
-        <v>1.794827222824097</v>
-      </c>
-    </row>
-    <row r="128" spans="1:3">
+        <v>1.7948272228240969</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128" s="1">
         <v>45274</v>
       </c>
@@ -1772,7 +1793,7 @@
         <v>2.02956223487854</v>
       </c>
     </row>
-    <row r="129" spans="1:3">
+    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129" s="1">
         <v>45274</v>
       </c>
@@ -1780,10 +1801,10 @@
         <v>7</v>
       </c>
       <c r="C129">
-        <v>2.961165428161621</v>
-      </c>
-    </row>
-    <row r="130" spans="1:3">
+        <v>2.9611654281616211</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130" s="1">
         <v>45274</v>
       </c>
@@ -1791,10 +1812,10 @@
         <v>8</v>
       </c>
       <c r="C130">
-        <v>3.275029420852661</v>
-      </c>
-    </row>
-    <row r="131" spans="1:3">
+        <v>3.2750294208526611</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A131" s="1">
         <v>45274</v>
       </c>
@@ -1805,7 +1826,7 @@
         <v>2.898346900939941</v>
       </c>
     </row>
-    <row r="132" spans="1:3">
+    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132" s="1">
         <v>45274</v>
       </c>
@@ -1813,10 +1834,10 @@
         <v>10</v>
       </c>
       <c r="C132">
-        <v>2.649399280548096</v>
-      </c>
-    </row>
-    <row r="133" spans="1:3">
+        <v>2.6493992805480961</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133" s="1">
         <v>45274</v>
       </c>
@@ -1827,7 +1848,7 @@
         <v>2.917227983474731</v>
       </c>
     </row>
-    <row r="134" spans="1:3">
+    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134" s="1">
         <v>45274</v>
       </c>
@@ -1835,10 +1856,10 @@
         <v>12</v>
       </c>
       <c r="C134">
-        <v>3.260042905807495</v>
-      </c>
-    </row>
-    <row r="135" spans="1:3">
+        <v>3.2600429058074951</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A135" s="1">
         <v>45274</v>
       </c>
@@ -1849,7 +1870,7 @@
         <v>3.300528764724731</v>
       </c>
     </row>
-    <row r="136" spans="1:3">
+    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136" s="1">
         <v>45274</v>
       </c>
@@ -1860,7 +1881,7 @@
         <v>3.06734299659729</v>
       </c>
     </row>
-    <row r="137" spans="1:3">
+    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A137" s="1">
         <v>45274</v>
       </c>
@@ -1868,10 +1889,10 @@
         <v>15</v>
       </c>
       <c r="C137">
-        <v>2.990092754364014</v>
-      </c>
-    </row>
-    <row r="138" spans="1:3">
+        <v>2.9900927543640141</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A138" s="1">
         <v>45274</v>
       </c>
@@ -1879,10 +1900,10 @@
         <v>16</v>
       </c>
       <c r="C138">
-        <v>2.243174076080322</v>
-      </c>
-    </row>
-    <row r="139" spans="1:3">
+        <v>2.2431740760803218</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A139" s="1">
         <v>45274</v>
       </c>
@@ -1890,10 +1911,10 @@
         <v>17</v>
       </c>
       <c r="C139">
-        <v>2.589770317077637</v>
-      </c>
-    </row>
-    <row r="140" spans="1:3">
+        <v>2.5897703170776372</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A140" s="1">
         <v>45274</v>
       </c>
@@ -1901,10 +1922,10 @@
         <v>18</v>
       </c>
       <c r="C140">
-        <v>2.630655288696289</v>
-      </c>
-    </row>
-    <row r="141" spans="1:3">
+        <v>2.6306552886962891</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A141" s="1">
         <v>45274</v>
       </c>
@@ -1915,7 +1936,7 @@
         <v>2.475153923034668</v>
       </c>
     </row>
-    <row r="142" spans="1:3">
+    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A142" s="1">
         <v>45274</v>
       </c>
@@ -1923,10 +1944,10 @@
         <v>20</v>
       </c>
       <c r="C142">
-        <v>2.549089431762695</v>
-      </c>
-    </row>
-    <row r="143" spans="1:3">
+        <v>2.5490894317626949</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A143" s="1">
         <v>45274</v>
       </c>
@@ -1937,7 +1958,7 @@
         <v>2.177978515625</v>
       </c>
     </row>
-    <row r="144" spans="1:3">
+    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A144" s="1">
         <v>45274</v>
       </c>
@@ -1948,7 +1969,7 @@
         <v>1.639663934707642</v>
       </c>
     </row>
-    <row r="145" spans="1:3">
+    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A145" s="1">
         <v>45274</v>
       </c>
@@ -1956,7 +1977,7 @@
         <v>23</v>
       </c>
       <c r="C145">
-        <v>0.9765159487724304</v>
+        <v>0.97651594877243042</v>
       </c>
     </row>
   </sheetData>

</xml_diff>